<commit_message>
Finish Week 2 and quiz for Stanford ML
</commit_message>
<xml_diff>
--- a/MachineLearning/Coursera/StanfordMachineLearning/MultivariateLinearRegression.xlsx
+++ b/MachineLearning/Coursera/StanfordMachineLearning/MultivariateLinearRegression.xlsx
@@ -453,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -464,7 +464,7 @@
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33.75" thickBot="1">
+    <row r="1" spans="1:3" ht="17.25" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +578,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <f t="shared" ref="A12:C14" si="1">A3-$A$7</f>
+        <f t="shared" ref="A12:A14" si="1">A3-$A$7</f>
         <v>-9</v>
       </c>
       <c r="B12">
@@ -624,7 +624,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16">
+      <c r="A16" s="3">
         <f>A11/$A$9</f>
         <v>0.32</v>
       </c>
@@ -639,7 +639,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <f t="shared" ref="A17:C19" si="4">A12/$A$9</f>
+        <f t="shared" ref="A17:A19" si="4">A12/$A$9</f>
         <v>-0.36</v>
       </c>
       <c r="B17" s="3">

</xml_diff>